<commit_message>
Make some updates and implement the script on the server
</commit_message>
<xml_diff>
--- a/p0033-DxValue.xlsx
+++ b/p0033-DxValue.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cassie/Dropbox/GA/Website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3B89C7-7F5B-5C40-BB84-433BD77A8247}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A183FE3E-B0F2-DB45-85D5-3A91982912F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{E797EA7B-D86F-E44F-A89B-DF9525C72BBA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" xr2:uid="{E797EA7B-D86F-E44F-A89B-DF9525C72BBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -544,12 +544,13 @@
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="6" max="6" width="8.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
     <col min="11" max="11" width="17.6640625" customWidth="1"/>

</xml_diff>